<commit_message>
update api product priceListed
</commit_message>
<xml_diff>
--- a/ProductUploadTemplate.xlsx
+++ b/ProductUploadTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chuyen-nganh\Capstone\p\p\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieunguyen/Desktop/Git/SavingHourMarket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD14CF1-A4C6-4508-AE8C-0968B1C985E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A1A2FE-53BB-9B48-85E9-5DCA7AC88260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="456" windowWidth="17280" windowHeight="11784" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin sản phẩm" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>STT</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Dưa hấu đỏ 1kg</t>
+  </si>
+  <si>
+    <t>Giá niêm yết</t>
   </si>
 </sst>
 </file>
@@ -600,28 +603,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC28846-1426-B243-8590-7161B15BFA22}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K2" sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.19921875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="49.69921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="12.69921875" style="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -631,29 +636,32 @@
       <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -663,29 +671,32 @@
       <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="17">
+        <v>50000</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16">
+      <c r="H2" s="16">
         <v>45311</v>
       </c>
-      <c r="H2" s="17">
+      <c r="I2" s="17">
         <v>30000</v>
       </c>
-      <c r="I2" s="17">
+      <c r="J2" s="17">
         <v>21000</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -695,29 +706,32 @@
       <c r="C3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="17">
+        <v>30000</v>
+      </c>
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="16">
+      <c r="H3" s="16">
         <v>45301</v>
       </c>
-      <c r="H3" s="17">
+      <c r="I3" s="17">
         <v>25000</v>
       </c>
-      <c r="I3" s="17">
+      <c r="J3" s="17">
         <v>20000</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -727,29 +741,32 @@
       <c r="C4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17">
+        <v>30000</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="16">
+      <c r="H4" s="16">
         <v>45311</v>
       </c>
-      <c r="H4" s="17">
+      <c r="I4" s="17">
         <v>20000</v>
       </c>
-      <c r="I4" s="17">
+      <c r="J4" s="17">
         <v>10000</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="K4" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>5</v>
       </c>
@@ -759,29 +776,31 @@
       <c r="C5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="17">
+        <v>40000</v>
+      </c>
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="16">
+      <c r="H5" s="16">
         <v>45306</v>
       </c>
-      <c r="H5" s="17">
+      <c r="I5" s="17">
         <v>30000</v>
       </c>
-      <c r="I5" s="17">
+      <c r="J5" s="17">
         <v>20000</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="K5" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -797,22 +816,22 @@
       <selection activeCell="I2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="50.296875" customWidth="1"/>
-    <col min="10" max="10" width="112.69921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.796875" customWidth="1"/>
+    <col min="9" max="9" width="50.33203125" customWidth="1"/>
+    <col min="10" max="10" width="112.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -844,7 +863,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
@@ -876,7 +895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -908,7 +927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -938,7 +957,7 @@
       </c>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -967,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
update api getOrderBatch-Tframe and upload excel product
</commit_message>
<xml_diff>
--- a/ProductUploadTemplate.xlsx
+++ b/ProductUploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieunguyen/Desktop/Git/SavingHourMarket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A1A2FE-53BB-9B48-85E9-5DCA7AC88260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8061451D-C2EF-EB4C-8B49-F4CF1B0F027A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="32880" windowHeight="19540" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin sản phẩm" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -53,42 +53,12 @@
     <t>Mô tả sản phẩm</t>
   </si>
   <si>
-    <t>Sữa Chua Hảo Hạn</t>
-  </si>
-  <si>
-    <t>Rất ngon bổ dưỡng</t>
-  </si>
-  <si>
-    <t>Kem nền</t>
-  </si>
-  <si>
-    <t>Chăm sóc da</t>
-  </si>
-  <si>
-    <t>Cơm cuộn Nhật Bản</t>
-  </si>
-  <si>
-    <t>Rất ngon nhưng không bổ dưỡng lắm</t>
-  </si>
-  <si>
-    <t>Cơm cuộn Hàn Quốc</t>
-  </si>
-  <si>
     <t>Vinmart+</t>
   </si>
   <si>
-    <t>Co.opmart</t>
-  </si>
-  <si>
-    <t>Satrafoods</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trái    cây  </t>
   </si>
   <si>
-    <t>Mỹ phẩm</t>
-  </si>
-  <si>
     <t>Siêu thị</t>
   </si>
   <si>
@@ -98,13 +68,7 @@
     <t>HSD</t>
   </si>
   <si>
-    <t>34 Đ. Nam Cao, Phường Tân Phú, Quận 9, Hồ Chí Minh</t>
-  </si>
-  <si>
     <t>Địa chỉ kho lưu giữ + số lượng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34 Đ. Nam Cao, Phường Tân Phú, Quận 9, Hồ Chí Minh;30 </t>
   </si>
   <si>
     <t>34 Đ. Nam Cao, Phường Tân Phú, Quận 9, Hồ Chí Minh;30 
@@ -117,9 +81,6 @@
     <t>TH1: Lô sản phẩm có cùng HSD nhưng có nhiều kho lưu trữ khác nhau (mỗi địa chỉ siêu thị ứng với số lượng sp lưu trữ phải ở riêng 1 dòng trong 1 ô thì hệ thống mới truy suất đc thông tin</t>
   </si>
   <si>
-    <t>TH2: Lô sản phẩm có cùng Tên, Mô tả, Danh mục với lô sản phẩm ở trên nhưng có HSD, Giá bán, Giá gốc khác sẽ được coi là lô khác của cùng 1 sản phẩm (Nếu một trong những thông tin của các mục -Tên, Mô tả, Danh mục phụ, Siêu thị - khác nhau sẽ được hệ thống coi là 1 sản phẩm khác )</t>
-  </si>
-  <si>
     <t>34 Đ. Nam Cao, Phường Tân Phú, Quận 9, Hồ Chí Minh;31</t>
   </si>
   <si>
@@ -157,6 +118,15 @@
   </si>
   <si>
     <t>Giá niêm yết</t>
+  </si>
+  <si>
+    <t>Hình ảnh</t>
+  </si>
+  <si>
+    <t>TH2: Lô sản phẩm có cùng Tên, Mô tả, Danh mục phụ, Đơn vị, Giá niêm yết với lô sản phẩm ở trên nhưng có HSD, Giá bán, Giá gốc khác sẽ được coi là lô khác của cùng 1 sản phẩm (Nếu một trong những thông tin của các mục -Tên, Mô tả, Danh mục phụ, Siêu thị - khác nhau sẽ được hệ thống coi là 1 sản phẩm khác )</t>
+  </si>
+  <si>
+    <t>Lưu ý :Lưu ý lô hàng của các sản phẩm phải khác nhau về HSD, nếu cùng HSD phải nhập thông tin trên cùng 1 dòng.  Nếu sản phẩm ở hai hàng nếu giống nhau về Tên, Mô tả, Danh mục phụ, Đơn vị, Giá niêm yết với sản phẩm  và có cùng HSD, Giá bán, Giá gốc giống nhau sẽ được coi là lô khác của cùng 1 sản phẩm và lúc này hệ thống sẽ báo lỗi.</t>
   </si>
 </sst>
 </file>
@@ -229,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,48 +216,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -304,6 +273,544 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1733550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E42EA8F-8B6F-45A5-DC9E-0A8AE5BC2340}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13944600" y="6261100"/>
+          <a:ext cx="2209800" cy="1657350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2429935</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1651001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A84F694-AC75-9D89-B3D0-879112F4D5A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13982700" y="460375"/>
+          <a:ext cx="2163235" cy="1622426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1593850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DC9E63A-83BD-E834-2DF2-544C24CC6777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14058900" y="4610100"/>
+          <a:ext cx="1752600" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2294467</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1676400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF99934-1577-B1C5-C7FE-F29BA2167016}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16903700" y="635000"/>
+          <a:ext cx="1964267" cy="1473200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>508001</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>250825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2235200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1685925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB50F2C-DE53-D409-337D-77CD3EF2B653}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22148801" y="682625"/>
+          <a:ext cx="1727199" cy="1435100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>436033</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2484967</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1739900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{310A2DAD-D9EA-35AA-6D2E-C615D431D40F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14152033" y="2514600"/>
+          <a:ext cx="2048934" cy="1536700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>2501900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1838324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D5C6F5E-DB31-45EC-5831-33501CAB01EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16738600" y="4416424"/>
+          <a:ext cx="2336800" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>187324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2273300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1739899</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB1439D2-0D59-AAE9-2813-D978305F0879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19354800" y="4518024"/>
+          <a:ext cx="2070100" cy="1552575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1733550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628A2536-9E9D-2B40-8662-F1FAB21FC6F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13944600" y="6692900"/>
+          <a:ext cx="2209800" cy="1657350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2120900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1828800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10A8D506-87A4-284A-A236-AD915B07C543}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13970000" y="561975"/>
+          <a:ext cx="1866900" cy="1698625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2095500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1593850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4E3D163-7DF1-7444-8EBF-A4BD23BF54D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14058900" y="5041900"/>
+          <a:ext cx="1752600" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>245532</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2666999</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1905000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{641FD802-4644-D048-8E06-EC3F18D7EDB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13961532" y="2832100"/>
+          <a:ext cx="2421467" cy="1816100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -603,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC28846-1426-B243-8590-7161B15BFA22}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="A1:K2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,216 +1129,232 @@
     <col min="9" max="9" width="7.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="49.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.6640625" style="1"/>
+    <col min="12" max="12" width="37.5" customWidth="1"/>
+    <col min="13" max="13" width="33.83203125" customWidth="1"/>
+    <col min="14" max="14" width="32.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5" style="1" customWidth="1"/>
+    <col min="16" max="16" width="33.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="D1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="17">
+        <v>17</v>
+      </c>
+      <c r="D2" s="15">
         <v>50000</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>15</v>
+      <c r="E2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="16">
+        <v>5</v>
+      </c>
+      <c r="H2" s="18">
         <v>45311</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="15">
         <v>30000</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="15">
         <v>21000</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>23</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17">
-        <v>30000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="15">
+        <v>50000</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>20</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="16">
+        <v>5</v>
+      </c>
+      <c r="H3" s="18">
         <v>45301</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="15">
         <v>25000</v>
       </c>
-      <c r="J3" s="17">
+      <c r="J3" s="15">
         <v>20000</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="K3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="17">
+        <v>21</v>
+      </c>
+      <c r="D4" s="15">
         <v>30000</v>
       </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="16">
+      <c r="E4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="18">
         <v>45311</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="15">
         <v>20000</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="15">
         <v>10000</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="153" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="15">
+        <v>40000</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="17">
-        <v>40000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="16">
+      <c r="H5" s="18">
         <v>45306</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="15">
         <v>30000</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="15">
         <v>20000</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A8363E-09C6-6342-B44E-6751B21E9957}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A2:I2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" customWidth="1"/>
-    <col min="9" max="9" width="50.33203125" customWidth="1"/>
-    <col min="10" max="10" width="112.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="49.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.5" customWidth="1"/>
+    <col min="13" max="13" width="33.83203125" customWidth="1"/>
+    <col min="14" max="14" width="28.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="35.5" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -841,181 +1364,192 @@
       <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>18</v>
+      <c r="D1" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>24</v>
-      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="15">
+        <v>50000</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="16">
-        <v>45616</v>
-      </c>
-      <c r="G2" s="17">
-        <v>20000</v>
-      </c>
-      <c r="H2" s="17">
-        <v>10000</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>25</v>
-      </c>
+      <c r="H2" s="18">
+        <v>45311</v>
+      </c>
+      <c r="I2" s="15">
+        <v>30000</v>
+      </c>
+      <c r="J2" s="15">
+        <v>21000</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15">
+        <v>50000</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="16">
-        <v>45617</v>
-      </c>
-      <c r="G3" s="17">
-        <v>21000</v>
-      </c>
-      <c r="H3" s="17">
-        <v>11000</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>26</v>
-      </c>
+      <c r="H3" s="18">
+        <v>45301</v>
+      </c>
+      <c r="I3" s="15">
+        <v>25000</v>
+      </c>
+      <c r="J3" s="15">
+        <v>20000</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="146" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="16">
-        <v>45616</v>
-      </c>
-      <c r="G4" s="17">
+        <v>21</v>
+      </c>
+      <c r="D4" s="15">
+        <v>30000</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="18">
+        <v>45311</v>
+      </c>
+      <c r="I4" s="15">
         <v>20000</v>
       </c>
-      <c r="H4" s="17">
+      <c r="J4" s="15">
         <v>10000</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="18"/>
+      <c r="K4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="15">
+        <v>40000</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="18">
+        <v>45306</v>
+      </c>
+      <c r="I5" s="15">
+        <v>30000</v>
+      </c>
+      <c r="J5" s="15">
+        <v>20000</v>
+      </c>
+      <c r="K5" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="16">
-        <v>45617</v>
-      </c>
-      <c r="G5" s="17">
-        <v>20000</v>
-      </c>
-      <c r="H5" s="17">
-        <v>10000</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="16">
-        <v>45616</v>
-      </c>
-      <c r="G6" s="17">
-        <v>20000</v>
-      </c>
-      <c r="H6" s="17">
-        <v>10000</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update fix bug error excel
</commit_message>
<xml_diff>
--- a/ProductUploadTemplate.xlsx
+++ b/ProductUploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hieunguyen/Desktop/Git/SavingHourMarket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC22435-9A06-4649-9983-566BF611B2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD594A-786B-C245-8C58-C9A950961603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="0" windowWidth="32880" windowHeight="19540" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16740" xr2:uid="{E7CAA011-5120-3042-8D8B-428EEF3B6769}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin sản phẩm" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC28846-1426-B243-8590-7161B15BFA22}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,9 +1211,7 @@
       <c r="E5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>6</v>
-      </c>
+      <c r="F5" s="17"/>
       <c r="G5" s="19" t="s">
         <v>5</v>
       </c>

</xml_diff>